<commit_message>
Implemented code for sending media file
</commit_message>
<xml_diff>
--- a/9AC.xlsx
+++ b/9AC.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>message</t>
   </si>
@@ -30,19 +30,22 @@
     <t>Number</t>
   </si>
   <si>
-    <t>Brandon</t>
-  </si>
-  <si>
     <t>Hey (name) how are you, have a goodnight (name)</t>
   </si>
   <si>
-    <t>Mom</t>
+    <t>Aditi</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>D:\Products\Images\clothes.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -100,7 +103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -115,6 +118,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -175,7 +181,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -210,7 +216,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -387,18 +393,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C116"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:B22"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -406,10 +412,11 @@
     <col min="1" max="1" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.140625" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="5"/>
+    <col min="4" max="4" width="45.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1">
+    <row r="1" spans="1:4" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -419,177 +426,96 @@
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="30">
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="30">
       <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>7300836025</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
-        <v>7993061667</v>
+      <c r="D2" s="6" t="s">
+        <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="5">
-        <v>9885819739</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>7993061667</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="5">
-        <v>9885819739</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1">
-        <v>7993061667</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5">
-        <v>9885819739</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1">
-        <v>7993061667</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="5">
-        <v>9885819739</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1">
-        <v>7993061667</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="5">
-        <v>9885819739</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="1">
-        <v>7993061667</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="5">
-        <v>9885819739</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="1">
-        <v>7993061667</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="5">
-        <v>9885819739</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="1">
-        <v>7993061667</v>
-      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3"/>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3"/>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3"/>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3"/>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3"/>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3"/>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3"/>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="3"/>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="3"/>
+      <c r="B16" s="1"/>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="5">
-        <v>9885819739</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="1"/>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="1">
-        <v>7993061667</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="5">
-        <v>9885819739</v>
-      </c>
+      <c r="A18" s="3"/>
+      <c r="B18" s="1"/>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="1">
-        <v>7993061667</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="5">
-        <v>9885819739</v>
-      </c>
+      <c r="A20" s="3"/>
+      <c r="B20" s="1"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="1">
-        <v>7993061667</v>
-      </c>
+      <c r="A22" s="3"/>
+      <c r="B22" s="1"/>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="3"/>

</xml_diff>